<commit_message>
Funcionalidad de los 2 scripts ok -- prueba exitosa con el dis 04/02/2026
</commit_message>
<xml_diff>
--- a/excel_dentos/01_citas_detallado/Citas detallado FEBRERO 4.xlsx
+++ b/excel_dentos/01_citas_detallado/Citas detallado FEBRERO 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\automatizaciones\excelFormatos\excel_dentos\01_citas_detallado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B963D98-C6A4-4DA1-9ADE-40F404933811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB5422-64FE-4F9D-96E0-EBE5E2832AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B0159705-A2F1-4FDB-BE44-65E951BE45DF}"/>
   </bookViews>
@@ -1652,7 +1652,7 @@
         <v>44</v>
       </c>
       <c r="F6">
-        <v>10585509416</v>
+        <v>1058550941</v>
       </c>
       <c r="H6">
         <v>3126286658</v>

</xml_diff>